<commit_message>
tuesday Oct 24 90% done instructor to course course to instructor
</commit_message>
<xml_diff>
--- a/src/main/resources/Instructors.xlsx
+++ b/src/main/resources/Instructors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tajbidhasan/Desktop/CS248/Teacherslink/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D088E7-D03A-3E4C-9EAB-A2A475C02EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B4C5D1-DF16-FC47-AD38-042A1716C25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6980" windowWidth="28800" windowHeight="12220" xr2:uid="{0559E169-9BA0-46D3-BCA8-777899FEC08C}"/>
+    <workbookView xWindow="0" yWindow="4720" windowWidth="28800" windowHeight="12220" xr2:uid="{0559E169-9BA0-46D3-BCA8-777899FEC08C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -324,9 +324,6 @@
     <t>MAT001L MAT006 MAT007 MAT103 MAT111 MAT124 MAT131 MAT141 MAT142 MAT111L MAT125 MAT126 MAT210 MAT203 MAT205</t>
   </si>
   <si>
-    <t>MAT001L MAT006 MAT101 MAT103 MAT111 MAT124 MAT131 MAT141 MAT102 MAT111L MAT125 MAT126 MAT210 MAT203</t>
-  </si>
-  <si>
     <t>MAT001L MAT006 MAT007 MAT103 MAT111 MAT124 MAT102 MAT141 MAT142 MAT111L MAT141 MAT142 MAT210 MAT205 MAT104</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>MAT001L MAT006 MAT007 MAT103 MAT111 MAT124 MAT131 MAT141 MAT142 MAT111L MAT007L MAT009</t>
+  </si>
+  <si>
+    <t>MAT001L MAT006 MAT101 MAT103 MAT111 MAT124 MAT131 MAT141 MAT102 MAT111L MAT125 MAT126 MAT210 MAT203 MAT205</t>
   </si>
 </sst>
 </file>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35023B1C-0E6B-4AA4-92F2-D8F267FFE4E7}">
   <dimension ref="A1:O134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:K8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -880,7 +880,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -1302,7 +1302,7 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -1371,7 +1371,7 @@
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -1446,7 +1446,7 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -1515,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -1662,7 +1662,7 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -1734,7 +1734,7 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
@@ -1797,7 +1797,7 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
@@ -1860,7 +1860,7 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
@@ -1923,7 +1923,7 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
@@ -1986,7 +1986,7 @@
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
@@ -2127,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
@@ -2199,7 +2199,7 @@
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
@@ -2271,7 +2271,7 @@
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
@@ -2340,7 +2340,7 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
@@ -2412,7 +2412,7 @@
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
@@ -2484,7 +2484,7 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
@@ -2553,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="3:15" x14ac:dyDescent="0.2">

</xml_diff>